<commit_message>
Changes in documentation and other things
- Change of name of _about_ to README
- Modification of README
- Change of some folders location
</commit_message>
<xml_diff>
--- a/data/input/excel/loads/loads_1am.xlsx
+++ b/data/input/excel/loads/loads_1am.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nogueira_raf\Documents\GitHub\scripts_powerfactory\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nogueira_raf\Documents\GitHub\scripts_powerfactory\data\input\excel\loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
-    <t>Loads</t>
-  </si>
-  <si>
     <t>Active Power</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>0.0442469</t>
+  </si>
+  <si>
+    <t>Load Name</t>
   </si>
 </sst>
 </file>
@@ -504,9 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -517,189 +515,189 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>